<commit_message>
Revised version of testing spreadsheet added to project
</commit_message>
<xml_diff>
--- a/assets/images/MS2_Testing.xlsx
+++ b/assets/images/MS2_Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smeghen\Documents\Ste Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{778427EC-C153-45CE-BCF2-7A7697E3B0AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{342BE4F7-320D-49E4-A15D-4656986E1627}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="917" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="73">
   <si>
     <t>Test ID</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>When text box is selected for input the number keypad should appear</t>
+  </si>
+  <si>
+    <t>Text can be difficult to read on smaller screen with the clash of the background image, overcame by changing text colour and adjusting the opacity of the background colour of the jumbotron</t>
   </si>
 </sst>
 </file>
@@ -614,7 +617,28 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="219">
+  <dxfs count="222">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2488,7 +2512,7 @@
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -8107,255 +8131,255 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="E3:E13 E15:E24 E26:E44 E46:E48 E87:E1048576">
-    <cfRule type="cellIs" dxfId="218" priority="484" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="484" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="485" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="485" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="486" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="486" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52:E59 E73 E61:E64">
-    <cfRule type="cellIs" dxfId="215" priority="403" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="403" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="404" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="404" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="405" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="405" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="cellIs" dxfId="212" priority="388" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="388" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="389" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="389" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="390" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="390" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" dxfId="209" priority="373" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="373" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="374" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="374" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="375" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="375" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="206" priority="358" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="358" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="359" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="359" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="360" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="360" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74">
-    <cfRule type="cellIs" dxfId="203" priority="355" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="355" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="356" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="356" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="357" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="357" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E75">
-    <cfRule type="cellIs" dxfId="200" priority="352" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="352" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="199" priority="353" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="353" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="354" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="354" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76:E77 E83:E86">
-    <cfRule type="cellIs" dxfId="197" priority="349" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="349" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="350" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="350" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="195" priority="351" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="351" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78 E80:E82">
-    <cfRule type="cellIs" dxfId="194" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="197" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="198" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="199" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78 E80:E82">
-    <cfRule type="cellIs" dxfId="191" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="194" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="195" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="196" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="188" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="37" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="38" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="39" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="185" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="34" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="35" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="36" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="cellIs" dxfId="182" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="31" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="32" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="33" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E72">
-    <cfRule type="cellIs" dxfId="179" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="28" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="29" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="30" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E79">
-    <cfRule type="cellIs" dxfId="176" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="25" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="26" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="27" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" dxfId="173" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="22" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="23" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="24" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="170" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="19" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="20" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="167" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="16" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="17" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="18" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="164" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="13" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="14" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69:E70">
-    <cfRule type="cellIs" dxfId="161" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="10" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="11" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="12" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71">
-    <cfRule type="cellIs" dxfId="158" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="7" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="8" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71">
-    <cfRule type="cellIs" dxfId="155" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="4" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="152" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="1" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8381,7 +8405,7 @@
     <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -8514,7 +8538,7 @@
       <c r="F9" s="38"/>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35"/>
       <c r="B10" s="36" t="s">
         <v>21</v>
@@ -8526,9 +8550,11 @@
         <v>10</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="38"/>
+        <v>5</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>72</v>
+      </c>
       <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -13959,17 +13985,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3 E88:E1048576">
-    <cfRule type="cellIs" dxfId="149" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="118" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="119" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="120" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E79 E81:E83">
+    <cfRule type="cellIs" dxfId="149" priority="46" operator="equal">
+      <formula>"Pass With Problems"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="47" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="48" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
     <cfRule type="cellIs" dxfId="146" priority="43" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -13980,7 +14017,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
+  <conditionalFormatting sqref="E25">
     <cfRule type="cellIs" dxfId="143" priority="40" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -13991,7 +14028,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
+  <conditionalFormatting sqref="E45">
     <cfRule type="cellIs" dxfId="140" priority="37" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14002,7 +14039,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
+  <conditionalFormatting sqref="E73">
     <cfRule type="cellIs" dxfId="137" priority="34" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14013,7 +14050,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
+  <conditionalFormatting sqref="E80">
     <cfRule type="cellIs" dxfId="134" priority="31" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14024,7 +14061,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E80">
+  <conditionalFormatting sqref="E60">
     <cfRule type="cellIs" dxfId="131" priority="28" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14035,7 +14072,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E60">
+  <conditionalFormatting sqref="E67">
     <cfRule type="cellIs" dxfId="128" priority="25" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14046,7 +14083,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E67">
+  <conditionalFormatting sqref="E68">
     <cfRule type="cellIs" dxfId="125" priority="22" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14057,7 +14094,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
+  <conditionalFormatting sqref="E69">
     <cfRule type="cellIs" dxfId="122" priority="19" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14068,7 +14105,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+  <conditionalFormatting sqref="E70:E71">
     <cfRule type="cellIs" dxfId="119" priority="16" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14079,7 +14116,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E70:E71">
+  <conditionalFormatting sqref="E72">
     <cfRule type="cellIs" dxfId="116" priority="13" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14101,7 +14138,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E72">
+  <conditionalFormatting sqref="E66">
     <cfRule type="cellIs" dxfId="110" priority="7" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14112,18 +14149,18 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="107" priority="4" operator="equal">
+  <conditionalFormatting sqref="E4:E9 E15:E24 E26:E44 E46:E48 E11:E13">
+    <cfRule type="cellIs" dxfId="107" priority="73" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="74" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="75" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E13 E15:E24 E26:E44 E46:E48">
+  <conditionalFormatting sqref="E52:E59 E74 E62:E65">
     <cfRule type="cellIs" dxfId="104" priority="70" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14134,7 +14171,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E52:E59 E74 E62:E65">
+  <conditionalFormatting sqref="E49">
     <cfRule type="cellIs" dxfId="101" priority="67" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14145,7 +14182,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
+  <conditionalFormatting sqref="E50">
     <cfRule type="cellIs" dxfId="98" priority="64" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14156,7 +14193,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
+  <conditionalFormatting sqref="E51">
     <cfRule type="cellIs" dxfId="95" priority="61" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14167,7 +14204,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
+  <conditionalFormatting sqref="E75">
     <cfRule type="cellIs" dxfId="92" priority="58" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14178,7 +14215,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E75">
+  <conditionalFormatting sqref="E76">
     <cfRule type="cellIs" dxfId="89" priority="55" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14189,7 +14226,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E76">
+  <conditionalFormatting sqref="E77:E78 E84:E87">
     <cfRule type="cellIs" dxfId="86" priority="52" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14200,7 +14237,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E77:E78 E84:E87">
+  <conditionalFormatting sqref="E79 E81:E83">
     <cfRule type="cellIs" dxfId="83" priority="49" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
@@ -14211,25 +14248,25 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E79 E81:E83">
-    <cfRule type="cellIs" dxfId="80" priority="46" operator="equal">
+  <conditionalFormatting sqref="E61">
+    <cfRule type="cellIs" dxfId="80" priority="4" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E61">
-    <cfRule type="cellIs" dxfId="77" priority="1" operator="equal">
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14237,7 +14274,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B88:B680 B6:B13 B15:B24 B26:B44 B46:B65" xr:uid="{35A5A50A-F002-46B7-9875-BD12897E0A84}">
       <formula1>Testing_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E81:E680 E6:E13 E15:E24 E26:E44 E74:E79 E67:E72 E46:E65" xr:uid="{71462F39-B07D-4FCF-BBEB-8B4EE6EF791C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E81:E680 E46:E65 E15:E24 E26:E44 E74:E79 E67:E72 E6:E13" xr:uid="{71462F39-B07D-4FCF-BBEB-8B4EE6EF791C}">
       <formula1>Result</formula1>
     </dataValidation>
   </dataValidations>
@@ -14255,7 +14292,7 @@
     <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -14405,7 +14442,7 @@
       <c r="F10" s="38"/>
       <c r="G10" s="21"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="35"/>
       <c r="B11" s="36" t="s">
         <v>21</v>
@@ -14417,9 +14454,11 @@
         <v>10</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="38"/>
+        <v>5</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>72</v>
+      </c>
       <c r="G11" s="21"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -19835,277 +19874,277 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3 E88:E1048576">
-    <cfRule type="cellIs" dxfId="74" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="118" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="119" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="120" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E79 E81:E83">
-    <cfRule type="cellIs" dxfId="71" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="46" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="47" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="48" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E79 E81:E83">
-    <cfRule type="cellIs" dxfId="68" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="43" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="44" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="45" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="65" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="40" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="41" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="42" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="62" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="37" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="38" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="39" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="cellIs" dxfId="59" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="34" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="35" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="36" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73">
-    <cfRule type="cellIs" dxfId="56" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="31" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="32" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="33" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E80">
-    <cfRule type="cellIs" dxfId="53" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="28" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="29" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="30" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" dxfId="50" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="25" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="26" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="27" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="47" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="22" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="23" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="24" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="44" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="19" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="20" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="41" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="16" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="17" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="18" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70:E71">
-    <cfRule type="cellIs" dxfId="38" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="13" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="14" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="15" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E72">
-    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="11" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E72">
-    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E13 E15:E24 E26:E44 E46:E48">
-    <cfRule type="cellIs" dxfId="26" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="70" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="71" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="72" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52:E59 E74 E62:E65">
-    <cfRule type="cellIs" dxfId="23" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="67" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="68" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="69" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="cellIs" dxfId="20" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="64" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="65" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="66" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" dxfId="17" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="61" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="62" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="63" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="14" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="58" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="59" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="60" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E75">
-    <cfRule type="cellIs" dxfId="11" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="55" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="56" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="57" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="cellIs" dxfId="8" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="52" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="53" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="54" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77:E78 E84:E87">
-    <cfRule type="cellIs" dxfId="5" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="49" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="50" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="51" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Pass With Problems"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>